<commit_message>
fixed leading zeros bug & added implementations of RS, RV
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="RA_RECORD" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,8 @@
     <sheet name="RW_RECORD" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="RT_RECORD" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="RF_RECORD" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="RS_RECORD" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="RV_RECORD" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="174">
   <si>
     <t xml:space="preserve">Record Identifier</t>
   </si>
@@ -456,16 +458,107 @@
   </si>
   <si>
     <t xml:space="preserve">Number of RW Records</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxing Entity Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suffix </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional Code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reporting Period </t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Quarterly Unemployment Insurance Total Wages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Quarterly Unemployment Insurance Total Taxable Wages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Weeks Worked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date First Employed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date of Separation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Employer Account Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Taxable Wages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Income Tax Withheld</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other State Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tax Type Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local Taxable Wages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local Income Tax Withheld</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Control Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplemental Data 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplemental Data 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">023456789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01012022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12312022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06152022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supplemental Data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -509,11 +602,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -571,7 +659,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -604,10 +692,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -618,6 +702,18 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -699,13 +795,13 @@
   </sheetPr>
   <dimension ref="A1:AN3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.86"/>
@@ -716,7 +812,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="17.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="30.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="38.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="38.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="13.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="13.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="16.91"/>
@@ -1015,7 +1111,7 @@
       <c r="U3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="V3" s="7" t="s">
+      <c r="V3" s="5" t="s">
         <v>37</v>
       </c>
       <c r="W3" s="5" t="s">
@@ -1040,7 +1136,7 @@
       </c>
       <c r="AG3" s="5"/>
       <c r="AH3" s="5"/>
-      <c r="AI3" s="8" t="s">
+      <c r="AI3" s="7" t="s">
         <v>40</v>
       </c>
       <c r="AJ3" s="5"/>
@@ -1072,11 +1168,11 @@
   </sheetPr>
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.21"/>
@@ -1313,7 +1409,7 @@
       <c r="Y3" s="5" t="n">
         <v>3332221111</v>
       </c>
-      <c r="AB3" s="8" t="s">
+      <c r="AB3" s="7" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1338,11 +1434,11 @@
   </sheetPr>
   <dimension ref="A1:AW27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.87"/>
@@ -1351,7 +1447,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="35.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="33.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="33.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.52"/>
@@ -1367,7 +1463,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="25.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="26.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="29.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="29.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="27.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="30.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="0" width="11.52"/>
@@ -1523,151 +1619,151 @@
       </c>
     </row>
     <row r="2" s="5" customFormat="true" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="n">
+      <c r="A2" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="10" t="n">
+      <c r="B2" s="9" t="n">
         <v>9</v>
       </c>
       <c r="C2" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="D2" s="10" t="n">
-        <v>15</v>
-      </c>
-      <c r="E2" s="10" t="n">
+      <c r="D2" s="9" t="n">
+        <v>15</v>
+      </c>
+      <c r="E2" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="F2" s="10" t="n">
+      <c r="F2" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="G2" s="10" t="n">
+      <c r="G2" s="9" t="n">
         <v>22</v>
       </c>
-      <c r="H2" s="10" t="n">
+      <c r="H2" s="9" t="n">
         <v>22</v>
       </c>
-      <c r="I2" s="10" t="n">
+      <c r="I2" s="9" t="n">
         <v>22</v>
       </c>
-      <c r="J2" s="10" t="n">
+      <c r="J2" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="K2" s="10" t="n">
+      <c r="K2" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="L2" s="10" t="n">
+      <c r="L2" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="M2" s="10" t="n">
+      <c r="M2" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="N2" s="10" t="n">
+      <c r="N2" s="9" t="n">
         <v>23</v>
       </c>
-      <c r="O2" s="10" t="n">
-        <v>15</v>
-      </c>
-      <c r="P2" s="10" t="n">
+      <c r="O2" s="9" t="n">
+        <v>15</v>
+      </c>
+      <c r="P2" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="Q2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="R2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="S2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="T2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="U2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="V2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="W2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="X2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="Y2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="Z2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="AA2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="AB2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="AC2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="AD2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="AE2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="AF2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="AG2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="AH2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="AI2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="AJ2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="AK2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="AL2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="AM2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="AN2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="AO2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="AP2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="AQ2" s="10" t="n">
-        <v>11</v>
-      </c>
-      <c r="AR2" s="10" t="n">
+      <c r="Q2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="R2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="S2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="T2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="U2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="V2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="W2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="X2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="Y2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="Z2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="AA2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="AB2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="AC2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="AD2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="AF2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="AH2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="AI2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="AJ2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="AK2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="AL2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="AM2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="AN2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="AO2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="AP2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="AQ2" s="9" t="n">
+        <v>11</v>
+      </c>
+      <c r="AR2" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AS2" s="10" t="n">
+      <c r="AS2" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AT2" s="10" t="n">
+      <c r="AT2" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AU2" s="10" t="n">
+      <c r="AU2" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AV2" s="10" t="n">
+      <c r="AV2" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AW2" s="10" t="n">
+      <c r="AW2" s="9" t="n">
         <v>23</v>
       </c>
     </row>
@@ -1840,167 +1936,167 @@
       <c r="AW4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
+      <c r="E6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
+      <c r="E8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
+      <c r="E10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
+      <c r="E12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
+      <c r="E14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
+      <c r="E16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
+      <c r="E18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
+      <c r="E20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
+      <c r="E22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
+      <c r="E24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
+      <c r="E26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2021,10 +2117,10 @@
   <dimension ref="A1:AD2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="N17" activeCellId="0" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.31"/>
@@ -2252,10 +2348,10 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.88"/>
   </cols>
@@ -2287,6 +2383,458 @@
       <c r="D2" s="4" t="n">
         <v>496</v>
       </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AM4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="22.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="14.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="13.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="12.99"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="11" customFormat="true" ht="54" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="E2" s="9" t="n">
+        <v>15</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="G2" s="9" t="n">
+        <v>20</v>
+      </c>
+      <c r="H2" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="J2" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="K2" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="L2" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="M2" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="N2" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="O2" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="P2" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="R2" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="S2" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="T2" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="U2" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="V2" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="W2" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="X2" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y2" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z2" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA2" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AB2" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC2" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE2" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="AF2" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AG2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="AI2" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="AJ2" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AK2" s="4" t="n">
+        <v>75</v>
+      </c>
+      <c r="AL2" s="4" t="n">
+        <v>75</v>
+      </c>
+      <c r="AM2" s="4" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>54321</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="5" t="n">
+        <v>12345</v>
+      </c>
+      <c r="U3" s="5" t="n">
+        <v>800</v>
+      </c>
+      <c r="V3" s="5" t="n">
+        <v>800</v>
+      </c>
+      <c r="W3" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="X3" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y3" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="AD3" s="5" t="n">
+        <v>3823</v>
+      </c>
+      <c r="AE3" s="5" t="n">
+        <v>382.3</v>
+      </c>
+      <c r="AG3" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="AH3" s="5" t="n">
+        <v>3823</v>
+      </c>
+      <c r="AI3" s="5" t="n">
+        <v>19.12</v>
+      </c>
+    </row>
+    <row r="4" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>12345</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>987654321</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="U4" s="5" t="n">
+        <v>500</v>
+      </c>
+      <c r="V4" s="5" t="n">
+        <v>500</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="X4" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y4" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD4" s="5" t="n">
+        <v>100000</v>
+      </c>
+      <c r="AE4" s="5" t="n">
+        <v>10000</v>
+      </c>
+      <c r="AG4" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="AH4" s="5" t="n">
+        <v>100000</v>
+      </c>
+      <c r="AI4" s="5" t="n">
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.49"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>